<commit_message>
Attempt to develop box plot
</commit_message>
<xml_diff>
--- a/test/es_enemy_4.xlsx
+++ b/test/es_enemy_4.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>Time</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Individual_Gain</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -476,6 +481,9 @@
       <c r="E2" t="n">
         <v>978</v>
       </c>
+      <c r="F2" t="n">
+        <v>99.40000000000001</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -493,6 +501,9 @@
       <c r="E3" t="n">
         <v>978</v>
       </c>
+      <c r="F3" t="n">
+        <v>99.40000000000001</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -510,6 +521,9 @@
       <c r="E4" t="n">
         <v>978</v>
       </c>
+      <c r="F4" t="n">
+        <v>99.40000000000001</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -527,6 +541,9 @@
       <c r="E5" t="n">
         <v>978</v>
       </c>
+      <c r="F5" t="n">
+        <v>99.40000000000001</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -543,6 +560,9 @@
       </c>
       <c r="E6" t="n">
         <v>978</v>
+      </c>
+      <c r="F6" t="n">
+        <v>99.40000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>